<commit_message>
Criação do cadastro de gastos com água.
</commit_message>
<xml_diff>
--- a/Cronograma_Richard.xlsx
+++ b/Cronograma_Richard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBC7125D-9025-4932-B695-209EADC8EE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481E7FFC-E5A1-4673-BDF7-695FF6544C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,21 +110,12 @@
     <t>Video apresentando o projeto até o momento. Fontes e documentação  (GRAU B)</t>
   </si>
   <si>
-    <t>Richard Gehlen Castilhos</t>
-  </si>
-  <si>
     <t xml:space="preserve">    EnerSave - Sistema para registro e controle dos gastos (água/energia) e descarte de lixo</t>
   </si>
   <si>
     <t xml:space="preserve">Criação do banco de dados (Schema/Tabelas); HomePage básica do sistema; Menu de acesso às funcionalidades (Cadastros/Consultas/Gráficos) </t>
   </si>
   <si>
-    <t xml:space="preserve">Melhoria HomePage; Cadastro/Atualização/Exclusão dos gastos com energia; Consulta dos gastos com energia                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cadastro/Atualização/Exclusão dos gastos com água; Consulta do gasto com água;  Cadastro/Atualização/Exclusão do descarte de lixo; Consulta do descarte de lixo;                                   </t>
-  </si>
-  <si>
     <t xml:space="preserve">Controle de acesso aos cadastros (autenticação); Gráfico do descarte de lixo                                                  </t>
   </si>
   <si>
@@ -132,6 +123,15 @@
   </si>
   <si>
     <t xml:space="preserve">Gráfico dos gastos gerais (Energia/Água);  Filtros para exibição dos gráficos.                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melhoria HomePage; Cadastro/Atualização/Exclusão dos gastos com água; Consulta do gasto com água;                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadastro/Atualização/Exclusão dos gastos com energia; Consulta dos gastos com energia; Cadastro/Atualização/Exclusão do descarte de lixo; Consulta do descarte de lixo;                                   </t>
+  </si>
+  <si>
+    <t>Felipe Lourenci Buniatti, Gabriela Marini Maroni e Richard Gehlen Castilhos</t>
   </si>
 </sst>
 </file>
@@ -141,7 +141,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +186,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -348,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -437,6 +454,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1075,7 +1098,7 @@
   <dimension ref="B1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C6" sqref="C6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,7 +1149,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
@@ -1136,12 +1159,12 @@
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
+      <c r="C6" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
     </row>
     <row r="7" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C7" s="20"/>
@@ -1198,7 +1221,7 @@
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="25">
         <v>3</v>
@@ -1211,8 +1234,8 @@
         <v>14</v>
       </c>
       <c r="C12" s="14"/>
-      <c r="D12" s="15" t="s">
-        <v>30</v>
+      <c r="D12" s="32" t="s">
+        <v>32</v>
       </c>
       <c r="E12" s="26">
         <v>3</v>
@@ -1226,7 +1249,7 @@
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E13" s="26">
         <v>3</v>
@@ -1309,7 +1332,7 @@
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E21" s="25">
         <v>2</v>
@@ -1323,7 +1346,7 @@
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E22" s="25">
         <v>2.5</v>
@@ -1337,7 +1360,7 @@
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E23" s="26">
         <v>2.5</v>

</xml_diff>